<commit_message>
finish send admin answer
</commit_message>
<xml_diff>
--- a/src/reports/1422194909.xlsx
+++ b/src/reports/1422194909.xlsx
@@ -524,22 +524,22 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-10-17 10:21:12</t>
+          <t>2024-10-18 14:00:55</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Миронова Мирослава Григорьевна</t>
+          <t>Ntcn nt dsf</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>+79113152214</t>
+          <t>+7965214251</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>dog@gmail.com</t>
+          <t>asdaS@dasd.conm</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -549,22 +549,22 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>ываыва</t>
+          <t>sdf sdf</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>ыаврвар</t>
+          <t>sdgsfdgsdfg</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>01.11.2001</t>
+          <t>05.03.2024</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>7 месяца(ев)</t>
         </is>
       </c>
     </row>

</xml_diff>